<commit_message>
feat!: update sheets in file conductor_input.
New variables to get the coordinates of the barycenter of each defined conductor component:
    * X_barycenter
    * Y_barycenter
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_1_input.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_1_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/Description_of_Components/new_input_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C18CD829-1409-4491-A22A-8EABB4B857E7}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="13_ncr:1_{0BD40D79-8656-4BCB-943B-68FA050A86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD15AF16-C13E-4A87-98F1-0989E9B0A80C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="95">
   <si>
     <t>COSTETA</t>
   </si>
@@ -313,6 +313,18 @@
   </si>
   <si>
     <t xml:space="preserve">flag to show the real time plots of the maximum temperature jacket. Possible values True, False; defaults to True. </t>
+  </si>
+  <si>
+    <t>X_barycenter</t>
+  </si>
+  <si>
+    <t>x coordinate of the barycenter</t>
+  </si>
+  <si>
+    <t>Y_barycenter</t>
+  </si>
+  <si>
+    <t>y coordinate of the barycenter</t>
   </si>
 </sst>
 </file>
@@ -832,31 +844,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="3"/>
+    <col min="5" max="6" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="14">
-        <f>SUM(E$2:Z$2)</f>
+        <f>SUM(E$2:U$2)</f>
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -869,7 +881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="D2" s="4" t="s">
@@ -884,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
@@ -910,7 +922,7 @@
         <v>CHAN_2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -930,256 +942,296 @@
         <v>3.6965000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+      <c r="F6" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E8" s="20">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F8" s="20">
         <v>3.2676E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="24">
-        <v>0</v>
-      </c>
-      <c r="F7" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E10" s="21">
         <v>1</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F10" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E11" s="18">
         <v>1</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F11" s="18">
         <v>0.313</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E12" s="18">
         <v>-99</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F12" s="18">
         <v>-99</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E13" s="18">
         <v>0.02</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F13" s="18">
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="14" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="18" t="b">
+      <c r="E14" s="18" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F12" s="18" t="b">
+      <c r="F14" s="18" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="19">
-        <v>0</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="C15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="19">
+        <v>0</v>
+      </c>
+      <c r="F15" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="19">
-        <v>0</v>
-      </c>
-      <c r="F14" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="C16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="19">
+        <v>0</v>
+      </c>
+      <c r="F16" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E18" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F18" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="22" t="s">
+      <c r="B19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="22" t="b">
+      <c r="E19" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1192,31 +1244,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14:XFD14"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="3"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="14">
-        <f>SUM(E$2:Z2)</f>
+        <f>SUM(E$2:U2)</f>
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
@@ -1227,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1239,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1261,7 +1313,7 @@
         <v>STR_MIX_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1275,152 +1327,152 @@
         <v>40</v>
       </c>
       <c r="E4" s="23">
-        <f>(0.00052534+0.00025201)*E5</f>
+        <f>(0.00052534+0.00025201)*E7</f>
         <v>7.5395176499999997E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E7" s="24">
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E8" s="24">
         <v>2.0846</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E9" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E10" s="26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E11" s="26">
         <v>197.71</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="B12" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E12" s="21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B13" s="21" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="29">
-        <v>121508000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="29">
-        <v>32.35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>22</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>18</v>
@@ -1429,23 +1481,57 @@
         <v>80</v>
       </c>
       <c r="E13" s="29">
+        <v>121508000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="29">
+        <v>32.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="29">
         <v>16.22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="B16" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="22" t="b">
+      <c r="E16" s="22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1458,26 +1544,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCDFC4-8F8B-44BE-BC94-0C08DE31F1F6}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="3"/>
+    <col min="2" max="2" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
@@ -1493,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1505,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1527,7 +1613,7 @@
         <v>STR_SC_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1544,80 +1630,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E7" s="7">
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+    <row r="8" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="21" t="s">
+      <c r="B8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B9" s="21" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="29">
-        <v>170360000000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="21">
-        <v>30.23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>22</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>18</v>
@@ -1625,24 +1711,58 @@
       <c r="D9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="29">
+        <v>170360000000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="21">
+        <v>30.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="21">
         <v>16.73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="22" t="s">
+      <c r="B12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="22" t="b">
+      <c r="E12" s="22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1655,26 +1775,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD13407-BFB1-4787-A354-6C7A2E5E5AE6}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="1" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>36</v>
       </c>
@@ -1690,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1702,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1724,7 +1844,7 @@
         <v>STR_STAB_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1741,71 +1861,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E7" s="7">
         <v>0.96989999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E8" s="26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E9" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="B10" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="22" t="b">
+      <c r="E10" s="22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1818,26 +1972,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14:XFD14"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="1" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>17</v>
       </c>
@@ -1853,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1865,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1887,7 +2041,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1905,7 +2059,7 @@
         <v>3.0698999999999999E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1922,9 +2076,9 @@
         <v>2.7965999999999999E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>9</v>
@@ -1933,15 +2087,15 @@
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E6" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>9</v>
@@ -1950,125 +2104,159 @@
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="E9" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E10" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E12" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="6">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="22" t="s">
+      <c r="B14" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E14" s="27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="B15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E15" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="B16" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="22" t="b">
+      <c r="E16" s="22" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>